<commit_message>
Sewage generation per person and Installed capacity per person
</commit_message>
<xml_diff>
--- a/Data/CS Project Data.xlsx
+++ b/Data/CS Project Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://plakshauniversity1-my.sharepoint.com/personal/vishal_paudel_plaksha_edu_in/Documents/CS Project Sem1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="8_{5D3C63AA-D4D3-FD4D-A121-5063A3279D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49BE0248-EB9F-42DA-90BF-7BB22FE6744E}"/>
+  <xr:revisionPtr revIDLastSave="443" documentId="8_{5D3C63AA-D4D3-FD4D-A121-5063A3279D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7BB2D0D-9AC9-4172-9E00-D4BBA53F6F8F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20060" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20060" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Urban Population" sheetId="6" r:id="rId1"/>
     <sheet name="Population 2011" sheetId="10" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId3"/>
-    <sheet name="Sewage Telagana" sheetId="9" r:id="rId4"/>
-    <sheet name="Sewage Original" sheetId="11" r:id="rId5"/>
+    <sheet name="Graph1" sheetId="12" r:id="rId3"/>
+    <sheet name="Graph2" sheetId="13" r:id="rId4"/>
+    <sheet name="Sewage Telagana" sheetId="9" r:id="rId5"/>
+    <sheet name="Sewage Original" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Urban Population'!$L$1:$M$2</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="906">
   <si>
     <t>A - 2  DECADAL VARIATION  IN  POPULATION  SINCE  1901</t>
   </si>
@@ -2712,10 +2713,40 @@
 (in MLD)</t>
   </si>
   <si>
+    <t>Installed Capacity (in MLD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrepancy </t>
+  </si>
+  <si>
+    <t>States</t>
+  </si>
+  <si>
+    <t>Orissa</t>
+  </si>
+  <si>
+    <t>NCT of Delhi</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>Andaman             &amp;
+Nicobar Islands</t>
+  </si>
+  <si>
+    <t>Arunachal
+Pradesh</t>
+  </si>
+  <si>
+    <t>Dadra    &amp;    Nagar
+Haveli</t>
+  </si>
+  <si>
+    <t>Pondicherry</t>
+  </si>
+  <si>
     <t>States / UTs</t>
-  </si>
-  <si>
-    <t>Installed Capacity (in MLD)</t>
   </si>
   <si>
     <t>Proposed Capacity (in MLD)</t>
@@ -2724,27 +2755,6 @@
     <t>Total Treatment Capacity
 (in MLD) including
 planned / proposed</t>
-  </si>
-  <si>
-    <t>Andaman             &amp;
-Nicobar Islands</t>
-  </si>
-  <si>
-    <t>Arunachal
-Pradesh</t>
-  </si>
-  <si>
-    <t>Dadra    &amp;    Nagar
-Haveli</t>
-  </si>
-  <si>
-    <t>NCT of Delhi</t>
-  </si>
-  <si>
-    <t>Orissa</t>
-  </si>
-  <si>
-    <t>Pondicherry</t>
   </si>
   <si>
     <t>Total</t>
@@ -2793,7 +2803,7 @@
     </r>
   </si>
   <si>
-    <t>Telangana</t>
+    <t>Installed - Operational Treatment Capacity</t>
   </si>
 </sst>
 </file>
@@ -3218,6 +3228,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3239,7 +3250,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3610,15 +3620,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" customHeight="1">
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
       <c r="L1" t="s">
         <v>1</v>
       </c>
@@ -3642,10 +3652,10 @@
       <c r="E2" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="69"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="55" t="s">
         <v>9</v>
       </c>
@@ -3676,10 +3686,10 @@
         <v>14</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="70"/>
+      <c r="G3" s="71"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
       <c r="K3" s="1"/>
@@ -15120,10 +15130,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B64504-97D9-4562-987A-D2A2C4707683}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -15626,10 +15636,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
     <sortCondition descending="1" ref="B2:B35"/>
@@ -15639,6 +15645,557 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39554944-A632-491F-8873-DA07EE7B7E75}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C2:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="60">
+      <c r="A1" s="57" t="s">
+        <v>889</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>890</v>
+      </c>
+      <c r="C1" t="s">
+        <v>891</v>
+      </c>
+      <c r="D1" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="13.5">
+      <c r="A2" s="60">
+        <v>684</v>
+      </c>
+      <c r="B2" s="60">
+        <v>1839</v>
+      </c>
+      <c r="C2" s="67">
+        <f>B2-A2</f>
+        <v>1155</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.5">
+      <c r="A3" s="60">
+        <v>8</v>
+      </c>
+      <c r="B3" s="60">
+        <v>901</v>
+      </c>
+      <c r="C3" s="67">
+        <f>B3-A3</f>
+        <v>893</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.5">
+      <c r="A4" s="60">
+        <v>1922</v>
+      </c>
+      <c r="B4" s="60">
+        <v>2712</v>
+      </c>
+      <c r="C4" s="67">
+        <f>B4-A4</f>
+        <v>790</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5">
+      <c r="A5" s="60">
+        <v>337</v>
+      </c>
+      <c r="B5" s="60">
+        <v>897</v>
+      </c>
+      <c r="C5" s="67">
+        <f>B5-A5</f>
+        <v>560</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5">
+      <c r="A6" s="60">
+        <v>6366</v>
+      </c>
+      <c r="B6" s="60">
+        <v>6890</v>
+      </c>
+      <c r="C6" s="67">
+        <f>B6-A6</f>
+        <v>524</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5">
+      <c r="A7" s="60">
+        <f xml:space="preserve"> 443</f>
+        <v>443</v>
+      </c>
+      <c r="B7" s="60">
+        <f>833</f>
+        <v>833</v>
+      </c>
+      <c r="C7" s="67">
+        <f>B7-A7</f>
+        <v>390</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.5">
+      <c r="A8" s="60">
+        <v>55</v>
+      </c>
+      <c r="B8" s="60">
+        <v>378</v>
+      </c>
+      <c r="C8" s="67">
+        <f>B8-A8</f>
+        <v>323</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13.5">
+      <c r="A9" s="60">
+        <v>783</v>
+      </c>
+      <c r="B9" s="60">
+        <v>1086</v>
+      </c>
+      <c r="C9" s="67">
+        <f>B9-A9</f>
+        <v>303</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13.5">
+      <c r="A10" s="60">
+        <v>2715</v>
+      </c>
+      <c r="B10" s="60">
+        <v>2896</v>
+      </c>
+      <c r="C10" s="67">
+        <f>B10-A10</f>
+        <v>181</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.5">
+      <c r="A11" s="60">
+        <v>1601</v>
+      </c>
+      <c r="B11" s="60">
+        <v>1781</v>
+      </c>
+      <c r="C11" s="67">
+        <f>B11-A11</f>
+        <v>180</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.5">
+      <c r="A12" s="60">
+        <v>3224</v>
+      </c>
+      <c r="B12" s="60">
+        <v>3374</v>
+      </c>
+      <c r="C12" s="67">
+        <f>B12-A12</f>
+        <v>150</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.5">
+      <c r="A13" s="60">
+        <v>93</v>
+      </c>
+      <c r="B13" s="60">
+        <v>218</v>
+      </c>
+      <c r="C13" s="67">
+        <f>B13-A13</f>
+        <v>125</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13.5">
+      <c r="A14" s="60">
+        <v>345</v>
+      </c>
+      <c r="B14" s="60">
+        <v>448</v>
+      </c>
+      <c r="C14" s="67">
+        <f>B14-A14</f>
+        <v>103</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13.5">
+      <c r="A15" s="60">
+        <v>842</v>
+      </c>
+      <c r="B15" s="60">
+        <v>901</v>
+      </c>
+      <c r="C15" s="67">
+        <f>B15-A15</f>
+        <v>59</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5">
+      <c r="A16" s="60">
+        <v>99</v>
+      </c>
+      <c r="B16" s="60">
+        <v>136</v>
+      </c>
+      <c r="C16" s="67">
+        <f>B16-A16</f>
+        <v>37</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.5">
+      <c r="A17" s="60">
+        <v>271</v>
+      </c>
+      <c r="B17" s="60">
+        <v>293</v>
+      </c>
+      <c r="C17" s="67">
+        <f>B17-A17</f>
+        <v>22</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13.5">
+      <c r="A18" s="60">
+        <v>44</v>
+      </c>
+      <c r="B18" s="60">
+        <v>66</v>
+      </c>
+      <c r="C18" s="67">
+        <f>B18-A18</f>
+        <v>22</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13.5">
+      <c r="A19" s="60">
+        <v>3358</v>
+      </c>
+      <c r="B19" s="60">
+        <v>3378</v>
+      </c>
+      <c r="C19" s="67">
+        <f>B19-A19</f>
+        <v>20</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13.5">
+      <c r="A20" s="60">
+        <v>0</v>
+      </c>
+      <c r="B20" s="60">
+        <v>10</v>
+      </c>
+      <c r="C20" s="67">
+        <v>10</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="13.5">
+      <c r="A21" s="60">
+        <v>0</v>
+      </c>
+      <c r="B21" s="60">
+        <v>10</v>
+      </c>
+      <c r="C21" s="67">
+        <v>10</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13.5">
+      <c r="A22" s="60">
+        <v>114</v>
+      </c>
+      <c r="B22" s="60">
+        <v>120</v>
+      </c>
+      <c r="C22" s="67">
+        <v>6</v>
+      </c>
+      <c r="D22" s="59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="13.5">
+      <c r="A23" s="60">
+        <v>18</v>
+      </c>
+      <c r="B23" s="60">
+        <v>20</v>
+      </c>
+      <c r="C23" s="67">
+        <v>2</v>
+      </c>
+      <c r="D23" s="59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="27">
+      <c r="A24" s="60">
+        <v>0</v>
+      </c>
+      <c r="B24" s="60">
+        <v>0</v>
+      </c>
+      <c r="C24" s="67">
+        <f>A24-B24</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="27">
+      <c r="A25" s="60">
+        <v>0</v>
+      </c>
+      <c r="B25" s="60">
+        <v>0</v>
+      </c>
+      <c r="C25" s="67">
+        <v>0</v>
+      </c>
+      <c r="D25" s="59" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13.5">
+      <c r="A26" s="60">
+        <v>0</v>
+      </c>
+      <c r="B26" s="60">
+        <v>0</v>
+      </c>
+      <c r="C26" s="67">
+        <v>0</v>
+      </c>
+      <c r="D26" s="59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="13.5">
+      <c r="A27" s="60">
+        <v>73</v>
+      </c>
+      <c r="B27" s="60">
+        <v>73</v>
+      </c>
+      <c r="C27" s="67">
+        <f>B27-A27</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="27">
+      <c r="A28" s="60">
+        <v>24</v>
+      </c>
+      <c r="B28" s="60">
+        <v>24</v>
+      </c>
+      <c r="C28" s="67">
+        <v>0</v>
+      </c>
+      <c r="D28" s="59" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="13.5">
+      <c r="A29" s="60">
+        <v>1880</v>
+      </c>
+      <c r="B29" s="60">
+        <v>1880</v>
+      </c>
+      <c r="C29" s="67">
+        <f>B29-A29</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="13.5">
+      <c r="A30" s="60">
+        <v>22</v>
+      </c>
+      <c r="B30" s="60">
+        <v>22</v>
+      </c>
+      <c r="C30" s="67">
+        <v>0</v>
+      </c>
+      <c r="D30" s="59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="13.5">
+      <c r="A31" s="60">
+        <v>0</v>
+      </c>
+      <c r="B31" s="60">
+        <v>0</v>
+      </c>
+      <c r="C31" s="67">
+        <v>0</v>
+      </c>
+      <c r="D31" s="59" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13.5">
+      <c r="A32" s="60">
+        <v>0</v>
+      </c>
+      <c r="B32" s="60">
+        <v>0</v>
+      </c>
+      <c r="C32" s="67">
+        <v>0</v>
+      </c>
+      <c r="D32" s="59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="13.5">
+      <c r="A33" s="60">
+        <v>0</v>
+      </c>
+      <c r="B33" s="60">
+        <v>0</v>
+      </c>
+      <c r="C33" s="67">
+        <v>0</v>
+      </c>
+      <c r="D33" s="59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="13.5">
+      <c r="A34" s="60">
+        <v>0</v>
+      </c>
+      <c r="B34" s="60">
+        <v>0</v>
+      </c>
+      <c r="C34" s="67">
+        <v>0</v>
+      </c>
+      <c r="D34" s="59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="13.5">
+      <c r="A35" s="60">
+        <v>56</v>
+      </c>
+      <c r="B35" s="60">
+        <v>56</v>
+      </c>
+      <c r="C35" s="67">
+        <v>0</v>
+      </c>
+      <c r="D35" s="59" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="13.5">
+      <c r="A36" s="60">
+        <v>1492</v>
+      </c>
+      <c r="B36" s="60">
+        <v>1492</v>
+      </c>
+      <c r="C36" s="67">
+        <v>0</v>
+      </c>
+      <c r="D36" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D36">
+    <sortCondition descending="1" ref="C2:C36"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A4C575-3770-C14E-BF3B-7E3B14D66CAA}">
   <dimension ref="A1:F37"/>
   <sheetViews>
@@ -15656,19 +16213,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="59.1" customHeight="1">
       <c r="A1" s="56" t="s">
-        <v>890</v>
+        <v>900</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>888</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>893</v>
+        <v>902</v>
       </c>
       <c r="F1" s="57" t="s">
         <v>889</v>
@@ -15676,7 +16233,7 @@
     </row>
     <row r="2" spans="1:6" ht="27">
       <c r="A2" s="59" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="B2" s="60">
         <v>23</v>
@@ -15721,7 +16278,7 @@
     </row>
     <row r="4" spans="1:6" ht="27">
       <c r="A4" s="59" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="B4" s="60">
         <v>62</v>
@@ -15821,7 +16378,7 @@
     </row>
     <row r="9" spans="1:6" ht="27">
       <c r="A9" s="59" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="B9" s="60">
         <v>67</v>
@@ -16141,7 +16698,7 @@
     </row>
     <row r="25" spans="1:6" ht="13.5">
       <c r="A25" s="59" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="B25" s="60">
         <v>3330</v>
@@ -16161,7 +16718,7 @@
     </row>
     <row r="26" spans="1:6" ht="13.5">
       <c r="A26" s="59" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="B26" s="60">
         <v>1282</v>
@@ -16361,7 +16918,7 @@
     </row>
     <row r="36" spans="1:6" ht="15">
       <c r="A36" s="62" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="B36" s="63">
         <v>72368</v>
@@ -16380,14 +16937,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75" customHeight="1">
-      <c r="A37" s="71" t="s">
-        <v>901</v>
-      </c>
-      <c r="B37" s="72"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="73"/>
+      <c r="A37" s="72" t="s">
+        <v>904</v>
+      </c>
+      <c r="B37" s="73"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16397,12 +16954,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C27CB19-9475-A140-8B0D-57FD3A76FB35}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.95"/>
@@ -16410,29 +16967,32 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="105">
+    <row r="1" spans="1:7" ht="105">
       <c r="A1" s="56" t="s">
-        <v>890</v>
+        <v>900</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>888</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>893</v>
+        <v>902</v>
       </c>
       <c r="F1" s="57" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="60">
+      <c r="G1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60">
       <c r="A2" s="59" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="B2" s="60">
         <v>23</v>
@@ -16449,8 +17009,11 @@
       <c r="F2" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30">
+      <c r="G2" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="59" t="s">
         <v>16</v>
       </c>
@@ -16472,10 +17035,14 @@
         <f xml:space="preserve"> 443</f>
         <v>443</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30">
+      <c r="G3" s="67">
+        <f t="shared" ref="G3:G37" si="0" xml:space="preserve"> C3 - F3</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="59" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="B4" s="60">
         <v>62</v>
@@ -16492,8 +17059,12 @@
       <c r="F4" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
+      <c r="G4" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="59" t="s">
         <v>20</v>
       </c>
@@ -16512,8 +17083,12 @@
       <c r="F5" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15">
+      <c r="G5" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="59" t="s">
         <v>21</v>
       </c>
@@ -16532,8 +17107,12 @@
       <c r="F6" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15">
+      <c r="G6" s="67">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" s="59" t="s">
         <v>28</v>
       </c>
@@ -16552,8 +17131,12 @@
       <c r="F7" s="60">
         <v>271</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15">
+      <c r="G7" s="67">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="59" t="s">
         <v>31</v>
       </c>
@@ -16572,10 +17155,14 @@
       <c r="F8" s="60">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="45">
+      <c r="G8" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45">
       <c r="A9" s="59" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="B9" s="60">
         <v>67</v>
@@ -16592,8 +17179,12 @@
       <c r="F9" s="60">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15">
+      <c r="G9" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15">
       <c r="A10" s="59" t="s">
         <v>41</v>
       </c>
@@ -16612,8 +17203,12 @@
       <c r="F10" s="60">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15">
+      <c r="G10" s="67">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15">
       <c r="A11" s="59" t="s">
         <v>45</v>
       </c>
@@ -16632,8 +17227,12 @@
       <c r="F11" s="60">
         <v>3358</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15">
+      <c r="G11" s="67">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" s="59" t="s">
         <v>49</v>
       </c>
@@ -16652,8 +17251,12 @@
       <c r="F12" s="60">
         <v>1880</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="30">
+      <c r="G12" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="59" t="s">
         <v>52</v>
       </c>
@@ -16672,8 +17275,12 @@
       <c r="F13" s="60">
         <v>99</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="30">
+      <c r="G13" s="67">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30">
       <c r="A14" s="59" t="s">
         <v>56</v>
       </c>
@@ -16692,8 +17299,12 @@
       <c r="F14" s="60">
         <v>93</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
+      <c r="G14" s="67">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15">
       <c r="A15" s="59" t="s">
         <v>60</v>
       </c>
@@ -16712,8 +17323,12 @@
       <c r="F15" s="60">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15">
+      <c r="G15" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15">
       <c r="A16" s="59" t="s">
         <v>64</v>
       </c>
@@ -16732,8 +17347,12 @@
       <c r="F16" s="60">
         <v>1922</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15">
+      <c r="G16" s="67">
+        <f t="shared" si="0"/>
+        <v>790</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" s="59" t="s">
         <v>65</v>
       </c>
@@ -16752,8 +17371,12 @@
       <c r="F17" s="60">
         <v>114</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="30">
+      <c r="G17" s="67">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30">
       <c r="A18" s="59" t="s">
         <v>66</v>
       </c>
@@ -16772,8 +17395,12 @@
       <c r="F18" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="30">
+      <c r="G18" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30">
       <c r="A19" s="59" t="s">
         <v>68</v>
       </c>
@@ -16792,8 +17419,12 @@
       <c r="F19" s="60">
         <v>684</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15">
+      <c r="G19" s="67">
+        <f t="shared" si="0"/>
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15">
       <c r="A20" s="59" t="s">
         <v>71</v>
       </c>
@@ -16812,8 +17443,12 @@
       <c r="F20" s="60">
         <v>6366</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15">
+      <c r="G20" s="67">
+        <f t="shared" si="0"/>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15">
       <c r="A21" s="59" t="s">
         <v>73</v>
       </c>
@@ -16832,8 +17467,12 @@
       <c r="F21" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15">
+      <c r="G21" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15">
       <c r="A22" s="59" t="s">
         <v>76</v>
       </c>
@@ -16852,8 +17491,12 @@
       <c r="F22" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15">
+      <c r="G22" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15">
       <c r="A23" s="59" t="s">
         <v>79</v>
       </c>
@@ -16872,8 +17515,12 @@
       <c r="F23" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="15">
+      <c r="G23" s="67">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" s="59" t="s">
         <v>82</v>
       </c>
@@ -16892,10 +17539,14 @@
       <c r="F24" s="60">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="30">
+      <c r="G24" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30">
       <c r="A25" s="59" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="B25" s="60">
         <v>3330</v>
@@ -16912,10 +17563,14 @@
       <c r="F25" s="60">
         <v>2715</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15">
+      <c r="G25" s="67">
+        <f t="shared" si="0"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15">
       <c r="A26" s="59" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="B26" s="60">
         <v>1282</v>
@@ -16932,8 +17587,12 @@
       <c r="F26" s="60">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15">
+      <c r="G26" s="67">
+        <f t="shared" si="0"/>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15">
       <c r="A27" s="59" t="s">
         <v>899</v>
       </c>
@@ -16952,8 +17611,12 @@
       <c r="F27" s="60">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15">
+      <c r="G27" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15">
       <c r="A28" s="59" t="s">
         <v>93</v>
       </c>
@@ -16972,8 +17635,12 @@
       <c r="F28" s="60">
         <v>1601</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15">
+      <c r="G28" s="67">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15">
       <c r="A29" s="59" t="s">
         <v>96</v>
       </c>
@@ -16992,8 +17659,12 @@
       <c r="F29" s="60">
         <v>783</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15">
+      <c r="G29" s="67">
+        <f t="shared" si="0"/>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15">
       <c r="A30" s="59" t="s">
         <v>99</v>
       </c>
@@ -17012,8 +17683,12 @@
       <c r="F30" s="60">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15">
+      <c r="G30" s="67">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15">
       <c r="A31" s="59" t="s">
         <v>100</v>
       </c>
@@ -17032,10 +17707,14 @@
       <c r="F31" s="60">
         <v>1492</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15">
+      <c r="G31" s="67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15">
       <c r="A32" s="59" t="s">
-        <v>902</v>
+        <v>895</v>
       </c>
       <c r="B32" s="60">
         <v>2660</v>
@@ -17052,8 +17731,12 @@
       <c r="F32" s="60">
         <v>842</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15">
+      <c r="G32" s="67">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15">
       <c r="A33" s="59" t="s">
         <v>104</v>
       </c>
@@ -17072,8 +17755,12 @@
       <c r="F33" s="60">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="30">
+      <c r="G33" s="67">
+        <f t="shared" si="0"/>
+        <v>893</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30">
       <c r="A34" s="59" t="s">
         <v>107</v>
       </c>
@@ -17092,8 +17779,12 @@
       <c r="F34" s="60">
         <v>3224</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15">
+      <c r="G34" s="67">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15">
       <c r="A35" s="59" t="s">
         <v>110</v>
       </c>
@@ -17112,8 +17803,12 @@
       <c r="F35" s="60">
         <v>345</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15">
+      <c r="G35" s="67">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15">
       <c r="A36" s="59" t="s">
         <v>113</v>
       </c>
@@ -17132,10 +17827,14 @@
       <c r="F36" s="60">
         <v>337</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15">
+      <c r="G36" s="67">
+        <f t="shared" si="0"/>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15">
       <c r="A37" s="62" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="B37" s="63">
         <v>72368</v>
@@ -17152,16 +17851,20 @@
       <c r="F37" s="63">
         <v>26869</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="14.1">
-      <c r="A38" s="71" t="s">
-        <v>901</v>
-      </c>
-      <c r="B38" s="72"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="73"/>
+      <c r="G37" s="67">
+        <f t="shared" si="0"/>
+        <v>4972</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="14.1">
+      <c r="A38" s="72" t="s">
+        <v>904</v>
+      </c>
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>